<commit_message>
updated spf local data in baseline_iis
</commit_message>
<xml_diff>
--- a/models/baseline_iis/data/US_local.xlsx
+++ b/models/baseline_iis/data/US_local.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_no_core_rt/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/replication-hasenzagl-et-al-2021/models/baseline_iis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577C8393-8531-1E47-A4D8-A957AB1621B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3D3CBA-AB76-AC4F-A6AF-47B5742EC5AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="460" windowWidth="20920" windowHeight="16240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="6" r:id="rId1"/>
@@ -1994,10 +1994,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyymm"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -2120,9 +2119,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2466,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C444"/>
   <sheetViews>
-    <sheetView topLeftCell="A236" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -7313,7 +7314,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -7530,12 +7531,12 @@
       <c r="B19" s="2">
         <v>31137</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="18">
         <f>SPF_growth!K19/100</f>
         <v>9.2310923276235357E-3</v>
       </c>
-      <c r="D19" s="18">
-        <v>4.12</v>
+      <c r="D19" s="20">
+        <v>4.1242000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -7545,12 +7546,12 @@
       <c r="B20" s="2">
         <v>31228</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="18">
         <f>SPF_growth!K20/100</f>
         <v>8.0413554106493201E-3</v>
       </c>
-      <c r="D20" s="18">
-        <v>4.3499999999999996</v>
+      <c r="D20" s="20">
+        <v>4.3497000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -7560,12 +7561,12 @@
       <c r="B21" s="2">
         <v>31320</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="18">
         <f>SPF_growth!K21/100</f>
         <v>6.8305145354505825E-3</v>
       </c>
-      <c r="D21" s="18">
-        <v>4.25</v>
+      <c r="D21" s="20">
+        <v>4.2496999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -7575,12 +7576,12 @@
       <c r="B22" s="2">
         <v>31412</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="18">
         <f>SPF_growth!K22/100</f>
         <v>7.362304176079304E-3</v>
       </c>
-      <c r="D22" s="18">
-        <v>3.85</v>
+      <c r="D22" s="20">
+        <v>3.8496999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -7590,12 +7591,12 @@
       <c r="B23" s="2">
         <v>31502</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="18">
         <f>SPF_growth!K23/100</f>
         <v>6.972346001087093E-3</v>
       </c>
-      <c r="D23" s="18">
-        <v>3.59</v>
+      <c r="D23" s="20">
+        <v>3.5871</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -7605,12 +7606,12 @@
       <c r="B24" s="2">
         <v>31593</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="18">
         <f>SPF_growth!K24/100</f>
         <v>9.1249075773616184E-3</v>
       </c>
-      <c r="D24" s="18">
-        <v>3.41</v>
+      <c r="D24" s="20">
+        <v>3.4112</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -7620,12 +7621,12 @@
       <c r="B25" s="2">
         <v>31685</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="18">
         <f>SPF_growth!K25/100</f>
         <v>7.3248926246487489E-3</v>
       </c>
-      <c r="D25" s="18">
-        <v>3.5</v>
+      <c r="D25" s="20">
+        <v>3.4998999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -7635,12 +7636,12 @@
       <c r="B26" s="2">
         <v>31777</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="18">
         <f>SPF_growth!K26/100</f>
         <v>7.2429386776224902E-3</v>
       </c>
-      <c r="D26" s="18">
-        <v>3.62</v>
+      <c r="D26" s="20">
+        <v>3.6248</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -7650,12 +7651,12 @@
       <c r="B27" s="2">
         <v>31867</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="18">
         <f>SPF_growth!K27/100</f>
         <v>7.3186843382373468E-3</v>
       </c>
-      <c r="D27" s="18">
-        <v>3.9</v>
+      <c r="D27" s="20">
+        <v>3.8997000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -7665,12 +7666,12 @@
       <c r="B28" s="2">
         <v>31958</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="18">
         <f>SPF_growth!K28/100</f>
         <v>7.0498309407629467E-3</v>
       </c>
-      <c r="D28" s="18">
-        <v>4.3600000000000003</v>
+      <c r="D28" s="20">
+        <v>4.3624999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -7680,12 +7681,12 @@
       <c r="B29" s="2">
         <v>32050</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="18">
         <f>SPF_growth!K29/100</f>
         <v>7.0739588682282584E-3</v>
       </c>
-      <c r="D29" s="18">
-        <v>4.5</v>
+      <c r="D29" s="20">
+        <v>4.4999000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -7695,12 +7696,12 @@
       <c r="B30" s="2">
         <v>32142</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="18">
         <f>SPF_growth!K30/100</f>
         <v>5.4535653638578818E-3</v>
       </c>
-      <c r="D30" s="18">
-        <v>4.37</v>
+      <c r="D30" s="20">
+        <v>4.3749000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -7710,12 +7711,12 @@
       <c r="B31" s="2">
         <v>32233</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="18">
         <f>SPF_growth!K31/100</f>
         <v>5.3529086139807447E-3</v>
       </c>
-      <c r="D31" s="18">
-        <v>4.2</v>
+      <c r="D31" s="20">
+        <v>4.1997</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -7725,12 +7726,12 @@
       <c r="B32" s="2">
         <v>32324</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="18">
         <f>SPF_growth!K32/100</f>
         <v>6.6241501398442981E-3</v>
       </c>
-      <c r="D32" s="18">
-        <v>4.57</v>
+      <c r="D32" s="20">
+        <v>4.5749000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -7740,12 +7741,12 @@
       <c r="B33" s="2">
         <v>32416</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="18">
         <f>SPF_growth!K33/100</f>
         <v>6.5118259928413913E-3</v>
       </c>
-      <c r="D33" s="18">
-        <v>4.9800000000000004</v>
+      <c r="D33" s="20">
+        <v>4.9749999999999996</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -7755,11 +7756,11 @@
       <c r="B34" s="2">
         <v>32508</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="18">
         <f>SPF_growth!K34/100</f>
         <v>6.2972928794058358E-3</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="20">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -7770,12 +7771,12 @@
       <c r="B35" s="2">
         <v>32598</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="18">
         <f>SPF_growth!K35/100</f>
         <v>4.0494520061742367E-3</v>
       </c>
-      <c r="D35" s="18">
-        <v>4.8499999999999996</v>
+      <c r="D35" s="20">
+        <v>4.8498999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -7785,12 +7786,12 @@
       <c r="B36" s="2">
         <v>32689</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="18">
         <f>SPF_growth!K36/100</f>
         <v>3.812019316142834E-3</v>
       </c>
-      <c r="D36" s="18">
-        <v>4.91</v>
+      <c r="D36" s="20">
+        <v>4.9123000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -7800,11 +7801,11 @@
       <c r="B37" s="2">
         <v>32781</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="18">
         <f>SPF_growth!K37/100</f>
         <v>5.264785151075202E-3</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="20">
         <v>4.6500000000000004</v>
       </c>
     </row>
@@ -7815,12 +7816,12 @@
       <c r="B38" s="2">
         <v>32873</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="18">
         <f>SPF_growth!K38/100</f>
         <v>5.0121317528326603E-3</v>
       </c>
-      <c r="D38" s="18">
-        <v>4.2300000000000004</v>
+      <c r="D38" s="20">
+        <v>4.2249999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -7830,12 +7831,12 @@
       <c r="B39" s="2">
         <v>32963</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="18">
         <f>SPF_growth!K39/100</f>
         <v>5.774770227933379E-3</v>
       </c>
-      <c r="D39" s="18">
-        <v>4.3499999999999996</v>
+      <c r="D39" s="20">
+        <v>4.3498999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -7845,12 +7846,12 @@
       <c r="B40" s="2">
         <v>33054</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="18">
         <f>SPF_growth!K40/100</f>
         <v>6.2308049092900664E-3</v>
       </c>
-      <c r="D40" s="18">
-        <v>4.2</v>
+      <c r="D40" s="20">
+        <v>4.1997999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -7860,12 +7861,12 @@
       <c r="B41" s="2">
         <v>33146</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="18">
         <f>SPF_growth!K41/100</f>
         <v>2.9921486625135163E-3</v>
       </c>
-      <c r="D41" s="18">
-        <v>4.45</v>
+      <c r="D41" s="20">
+        <v>4.4493999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -7875,12 +7876,12 @@
       <c r="B42" s="2">
         <v>33238</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="18">
         <f>SPF_growth!K42/100</f>
         <v>1.8699840887628216E-3</v>
       </c>
-      <c r="D42" s="18">
-        <v>4.51</v>
+      <c r="D42" s="20">
+        <v>4.5114000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -7890,12 +7891,12 @@
       <c r="B43" s="2">
         <v>33328</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="18">
         <f>SPF_growth!K43/100</f>
         <v>4.9892985882478147E-3</v>
       </c>
-      <c r="D43" s="18">
-        <v>3.66</v>
+      <c r="D43" s="20">
+        <v>3.6623999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -7905,12 +7906,12 @@
       <c r="B44" s="2">
         <v>33419</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="18">
         <f>SPF_growth!K44/100</f>
         <v>6.7617243643305347E-3</v>
       </c>
-      <c r="D44" s="18">
-        <v>3.84</v>
+      <c r="D44" s="20">
+        <v>3.8374999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -7920,12 +7921,12 @@
       <c r="B45" s="2">
         <v>33511</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="18">
         <f>SPF_growth!K45/100</f>
         <v>7.0373174696498619E-3</v>
       </c>
-      <c r="D45" s="18">
-        <v>3.77</v>
+      <c r="D45" s="20">
+        <v>3.7724000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -7935,12 +7936,12 @@
       <c r="B46" s="2">
         <v>33603</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="18">
         <f>SPF_growth!K46/100</f>
         <v>7.0368503741999877E-3</v>
       </c>
-      <c r="D46" s="18">
-        <v>3.55</v>
+      <c r="D46" s="20">
+        <v>3.5499000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -7950,12 +7951,12 @@
       <c r="B47" s="2">
         <v>33694</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="18">
         <f>SPF_growth!K47/100</f>
         <v>7.0933774800152616E-3</v>
       </c>
-      <c r="D47" s="18">
-        <v>3.4</v>
+      <c r="D47" s="20">
+        <v>3.3999000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -7965,12 +7966,12 @@
       <c r="B48" s="2">
         <v>33785</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="18">
         <f>SPF_growth!K48/100</f>
         <v>7.8874483082800317E-3</v>
       </c>
-      <c r="D48" s="18">
-        <v>3.52</v>
+      <c r="D48" s="20">
+        <v>3.5249000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -7980,12 +7981,12 @@
       <c r="B49" s="2">
         <v>33877</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="18">
         <f>SPF_growth!K49/100</f>
         <v>6.7183843321154679E-3</v>
       </c>
-      <c r="D49" s="18">
-        <v>3.33</v>
+      <c r="D49" s="20">
+        <v>3.3250000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7995,12 +7996,12 @@
       <c r="B50" s="2">
         <v>33969</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="18">
         <f>SPF_growth!K50/100</f>
         <v>7.3995781607556488E-3</v>
       </c>
-      <c r="D50" s="18">
-        <v>3.25</v>
+      <c r="D50" s="20">
+        <v>3.2498999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -8010,12 +8011,12 @@
       <c r="B51" s="2">
         <v>34059</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="18">
         <f>SPF_growth!K51/100</f>
         <v>7.8185838971052135E-3</v>
       </c>
-      <c r="D51" s="18">
-        <v>3.21</v>
+      <c r="D51" s="20">
+        <v>3.2124999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -8025,12 +8026,12 @@
       <c r="B52" s="2">
         <v>34150</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="18">
         <f>SPF_growth!K52/100</f>
         <v>7.7060129398076604E-3</v>
       </c>
-      <c r="D52" s="18">
-        <v>3.37</v>
+      <c r="D52" s="20">
+        <v>3.3748999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -8040,11 +8041,11 @@
       <c r="B53" s="2">
         <v>34242</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="18">
         <f>SPF_growth!K53/100</f>
         <v>7.3623960000597233E-3</v>
       </c>
-      <c r="D53" s="18">
+      <c r="D53" s="20">
         <v>3.3</v>
       </c>
     </row>
@@ -8055,11 +8056,11 @@
       <c r="B54" s="2">
         <v>34334</v>
       </c>
-      <c r="C54" s="19">
+      <c r="C54" s="18">
         <f>SPF_growth!K54/100</f>
         <v>6.9373953182720882E-3</v>
       </c>
-      <c r="D54" s="18">
+      <c r="D54" s="20">
         <v>3.03</v>
       </c>
     </row>
@@ -8070,11 +8071,11 @@
       <c r="B55" s="2">
         <v>34424</v>
       </c>
-      <c r="C55" s="19">
+      <c r="C55" s="18">
         <f>SPF_growth!K55/100</f>
         <v>7.1121542451979547E-3</v>
       </c>
-      <c r="D55" s="18">
+      <c r="D55" s="20">
         <v>3.2</v>
       </c>
     </row>
@@ -8085,12 +8086,12 @@
       <c r="B56" s="2">
         <v>34515</v>
       </c>
-      <c r="C56" s="19">
+      <c r="C56" s="18">
         <f>SPF_growth!K56/100</f>
         <v>6.724734925990683E-3</v>
       </c>
-      <c r="D56" s="18">
-        <v>3.28</v>
+      <c r="D56" s="20">
+        <v>3.2749999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -8100,12 +8101,12 @@
       <c r="B57" s="2">
         <v>34607</v>
       </c>
-      <c r="C57" s="19">
+      <c r="C57" s="18">
         <f>SPF_growth!K57/100</f>
         <v>6.1874699511825781E-3</v>
       </c>
-      <c r="D57" s="18">
-        <v>3.33</v>
+      <c r="D57" s="20">
+        <v>3.3250000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -8115,12 +8116,12 @@
       <c r="B58" s="2">
         <v>34699</v>
       </c>
-      <c r="C58" s="19">
+      <c r="C58" s="18">
         <f>SPF_growth!K58/100</f>
         <v>6.3061654967608849E-3</v>
       </c>
-      <c r="D58" s="18">
-        <v>3.43</v>
+      <c r="D58" s="20">
+        <v>3.4249999999999998</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -8130,12 +8131,12 @@
       <c r="B59" s="2">
         <v>34789</v>
       </c>
-      <c r="C59" s="19">
+      <c r="C59" s="18">
         <f>SPF_growth!K59/100</f>
         <v>6.0623011217268985E-3</v>
       </c>
-      <c r="D59" s="18">
-        <v>3.41</v>
+      <c r="D59" s="20">
+        <v>3.4125000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -8145,12 +8146,12 @@
       <c r="B60" s="2">
         <v>34880</v>
       </c>
-      <c r="C60" s="19">
+      <c r="C60" s="18">
         <f>SPF_growth!K60/100</f>
         <v>6.331080545903145E-3</v>
       </c>
-      <c r="D60" s="18">
-        <v>3.53</v>
+      <c r="D60" s="20">
+        <v>3.5249999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -8160,12 +8161,12 @@
       <c r="B61" s="2">
         <v>34972</v>
       </c>
-      <c r="C61" s="19">
+      <c r="C61" s="18">
         <f>SPF_growth!K61/100</f>
         <v>6.7374799001742591E-3</v>
       </c>
-      <c r="D61" s="18">
-        <v>3.28</v>
+      <c r="D61" s="20">
+        <v>3.2749999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -8175,11 +8176,11 @@
       <c r="B62" s="2">
         <v>35064</v>
       </c>
-      <c r="C62" s="19">
+      <c r="C62" s="18">
         <f>SPF_growth!K62/100</f>
         <v>6.2437075477326243E-3</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D62" s="20">
         <v>2.95</v>
       </c>
     </row>
@@ -8190,12 +8191,12 @@
       <c r="B63" s="2">
         <v>35155</v>
       </c>
-      <c r="C63" s="19">
+      <c r="C63" s="18">
         <f>SPF_growth!K63/100</f>
         <v>5.9685755205713953E-3</v>
       </c>
-      <c r="D63" s="18">
-        <v>2.78</v>
+      <c r="D63" s="20">
+        <v>2.7749999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -8205,12 +8206,12 @@
       <c r="B64" s="2">
         <v>35246</v>
       </c>
-      <c r="C64" s="19">
+      <c r="C64" s="18">
         <f>SPF_growth!K64/100</f>
         <v>5.1061485916221727E-3</v>
       </c>
-      <c r="D64" s="18">
-        <v>2.87</v>
+      <c r="D64" s="20">
+        <v>2.8748999999999998</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -8220,12 +8221,12 @@
       <c r="B65" s="2">
         <v>35338</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="18">
         <f>SPF_growth!K65/100</f>
         <v>5.0873503970347844E-3</v>
       </c>
-      <c r="D65" s="18">
-        <v>3</v>
+      <c r="D65" s="20">
+        <v>3.0024999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -8235,12 +8236,12 @@
       <c r="B66" s="2">
         <v>35430</v>
       </c>
-      <c r="C66" s="19">
+      <c r="C66" s="18">
         <f>SPF_growth!K66/100</f>
         <v>5.4999064609069226E-3</v>
       </c>
-      <c r="D66" s="18">
-        <v>3.03</v>
+      <c r="D66" s="20">
+        <v>3.0249999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -8250,12 +8251,12 @@
       <c r="B67" s="2">
         <v>35520</v>
       </c>
-      <c r="C67" s="19">
+      <c r="C67" s="18">
         <f>SPF_growth!K67/100</f>
         <v>5.5436703808635635E-3</v>
       </c>
-      <c r="D67" s="18">
-        <v>3.06</v>
+      <c r="D67" s="20">
+        <v>3.0625</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -8265,12 +8266,12 @@
       <c r="B68" s="2">
         <v>35611</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C68" s="18">
         <f>SPF_growth!K68/100</f>
         <v>5.5060822588559599E-3</v>
       </c>
-      <c r="D68" s="18">
-        <v>3</v>
+      <c r="D68" s="20">
+        <v>2.9998999999999998</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -8280,12 +8281,12 @@
       <c r="B69" s="2">
         <v>35703</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="18">
         <f>SPF_growth!K69/100</f>
         <v>6.0934820113078825E-3</v>
       </c>
-      <c r="D69" s="18">
-        <v>2.85</v>
+      <c r="D69" s="20">
+        <v>2.8498999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -8295,11 +8296,11 @@
       <c r="B70" s="2">
         <v>35795</v>
       </c>
-      <c r="C70" s="19">
+      <c r="C70" s="18">
         <f>SPF_growth!K70/100</f>
         <v>5.8624505213646927E-3</v>
       </c>
-      <c r="D70" s="18">
+      <c r="D70" s="20">
         <v>2.6</v>
       </c>
     </row>
@@ -8310,12 +8311,12 @@
       <c r="B71" s="2">
         <v>35885</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="18">
         <f>SPF_growth!K71/100</f>
         <v>5.6184528476153073E-3</v>
       </c>
-      <c r="D71" s="18">
-        <v>2.2599999999999998</v>
+      <c r="D71" s="20">
+        <v>2.2624</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -8325,12 +8326,12 @@
       <c r="B72" s="2">
         <v>35976</v>
       </c>
-      <c r="C72" s="19">
+      <c r="C72" s="18">
         <f>SPF_growth!K72/100</f>
         <v>5.6124860919704034E-3</v>
       </c>
-      <c r="D72" s="18">
-        <v>2.4500000000000002</v>
+      <c r="D72" s="20">
+        <v>2.4499</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -8340,12 +8341,12 @@
       <c r="B73" s="2">
         <v>36068</v>
       </c>
-      <c r="C73" s="19">
+      <c r="C73" s="18">
         <f>SPF_growth!K73/100</f>
         <v>6.1870707036402184E-3</v>
       </c>
-      <c r="D73" s="18">
-        <v>2.48</v>
+      <c r="D73" s="20">
+        <v>2.4750000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -8355,12 +8356,12 @@
       <c r="B74" s="2">
         <v>36160</v>
       </c>
-      <c r="C74" s="19">
+      <c r="C74" s="18">
         <f>SPF_growth!K74/100</f>
         <v>4.6811346999353631E-3</v>
       </c>
-      <c r="D74" s="18">
-        <v>2.31</v>
+      <c r="D74" s="20">
+        <v>2.3123999999999998</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -8370,12 +8371,12 @@
       <c r="B75" s="2">
         <v>36250</v>
       </c>
-      <c r="C75" s="19">
+      <c r="C75" s="18">
         <f>SPF_growth!K75/100</f>
         <v>5.8747795233102806E-3</v>
       </c>
-      <c r="D75" s="18">
-        <v>2.17</v>
+      <c r="D75" s="20">
+        <v>2.1749000000000001</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -8385,11 +8386,11 @@
       <c r="B76" s="2">
         <v>36341</v>
       </c>
-      <c r="C76" s="19">
+      <c r="C76" s="18">
         <f>SPF_growth!K76/100</f>
         <v>6.4368840898705315E-3</v>
       </c>
-      <c r="D76" s="18">
+      <c r="D76" s="20">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -8400,12 +8401,12 @@
       <c r="B77" s="2">
         <v>36433</v>
       </c>
-      <c r="C77" s="19">
+      <c r="C77" s="18">
         <f>SPF_growth!K77/100</f>
         <v>6.3744641358740584E-3</v>
       </c>
-      <c r="D77" s="18">
-        <v>2.38</v>
+      <c r="D77" s="20">
+        <v>2.3786999999999998</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -8415,12 +8416,12 @@
       <c r="B78" s="2">
         <v>36525</v>
       </c>
-      <c r="C78" s="19">
+      <c r="C78" s="18">
         <f>SPF_growth!K78/100</f>
         <v>7.2807160968004769E-3</v>
       </c>
-      <c r="D78" s="18">
-        <v>2.5299999999999998</v>
+      <c r="D78" s="20">
+        <v>2.5249999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -8430,12 +8431,12 @@
       <c r="B79" s="2">
         <v>36616</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="18">
         <f>SPF_growth!K79/100</f>
         <v>7.5811621767614135E-3</v>
       </c>
-      <c r="D79" s="18">
-        <v>2.46</v>
+      <c r="D79" s="20">
+        <v>2.4624999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -8445,12 +8446,12 @@
       <c r="B80" s="2">
         <v>36707</v>
       </c>
-      <c r="C80" s="19">
+      <c r="C80" s="18">
         <f>SPF_growth!K80/100</f>
         <v>7.4056953353818233E-3</v>
       </c>
-      <c r="D80" s="18">
-        <v>2.61</v>
+      <c r="D80" s="20">
+        <v>2.6061999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -8460,12 +8461,12 @@
       <c r="B81" s="2">
         <v>36799</v>
       </c>
-      <c r="C81" s="19">
+      <c r="C81" s="18">
         <f>SPF_growth!K81/100</f>
         <v>7.5686105000138948E-3</v>
       </c>
-      <c r="D81" s="18">
-        <v>2.71</v>
+      <c r="D81" s="20">
+        <v>2.7124999999999999</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -8475,12 +8476,12 @@
       <c r="B82" s="2">
         <v>36891</v>
       </c>
-      <c r="C82" s="19">
+      <c r="C82" s="18">
         <f>SPF_growth!K82/100</f>
         <v>8.1499886860054715E-3</v>
       </c>
-      <c r="D82" s="18">
-        <v>2.68</v>
+      <c r="D82" s="20">
+        <v>2.6749999999999998</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -8490,12 +8491,12 @@
       <c r="B83" s="2">
         <v>36981</v>
       </c>
-      <c r="C83" s="19">
+      <c r="C83" s="18">
         <f>SPF_growth!K83/100</f>
         <v>8.0175650744016558E-3</v>
       </c>
-      <c r="D83" s="18">
-        <v>2.4900000000000002</v>
+      <c r="D83" s="20">
+        <v>2.4874999999999998</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -8505,12 +8506,12 @@
       <c r="B84" s="2">
         <v>37072</v>
       </c>
-      <c r="C84" s="19">
+      <c r="C84" s="18">
         <f>SPF_growth!K84/100</f>
         <v>7.0238949003273987E-3</v>
       </c>
-      <c r="D84" s="18">
-        <v>2.5099999999999998</v>
+      <c r="D84" s="20">
+        <v>2.5125000000000002</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -8520,11 +8521,11 @@
       <c r="B85" s="2">
         <v>37164</v>
       </c>
-      <c r="C85" s="19">
+      <c r="C85" s="18">
         <f>SPF_growth!K85/100</f>
         <v>7.7367802883900882E-3</v>
       </c>
-      <c r="D85" s="18">
+      <c r="D85" s="20">
         <v>2.6</v>
       </c>
     </row>
@@ -8535,12 +8536,12 @@
       <c r="B86" s="2">
         <v>37256</v>
       </c>
-      <c r="C86" s="19">
+      <c r="C86" s="18">
         <f>SPF_growth!K86/100</f>
         <v>6.2989332866600911E-3</v>
       </c>
-      <c r="D86" s="18">
-        <v>2.15</v>
+      <c r="D86" s="20">
+        <v>2.1497999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -8550,12 +8551,12 @@
       <c r="B87" s="2">
         <v>37346</v>
       </c>
-      <c r="C87" s="19">
+      <c r="C87" s="18">
         <f>SPF_growth!K87/100</f>
         <v>8.2056296806840567E-3</v>
       </c>
-      <c r="D87" s="18">
-        <v>2.2000000000000002</v>
+      <c r="D87" s="20">
+        <v>2.1999</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -8565,12 +8566,12 @@
       <c r="B88" s="2">
         <v>37437</v>
       </c>
-      <c r="C88" s="19">
+      <c r="C88" s="18">
         <f>SPF_growth!K88/100</f>
         <v>8.5999403513785655E-3</v>
       </c>
-      <c r="D88" s="18">
-        <v>2.35</v>
+      <c r="D88" s="20">
+        <v>2.3498999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -8580,12 +8581,12 @@
       <c r="B89" s="2">
         <v>37529</v>
       </c>
-      <c r="C89" s="19">
+      <c r="C89" s="18">
         <f>SPF_growth!K89/100</f>
         <v>7.9870220883944132E-3</v>
       </c>
-      <c r="D89" s="18">
-        <v>2.29</v>
+      <c r="D89" s="20">
+        <v>2.2873999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -8595,12 +8596,12 @@
       <c r="B90" s="2">
         <v>37621</v>
       </c>
-      <c r="C90" s="19">
+      <c r="C90" s="18">
         <f>SPF_growth!K90/100</f>
         <v>8.1614694367966312E-3</v>
       </c>
-      <c r="D90" s="18">
-        <v>2.19</v>
+      <c r="D90" s="20">
+        <v>2.1875</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -8610,12 +8611,12 @@
       <c r="B91" s="2">
         <v>37711</v>
       </c>
-      <c r="C91" s="19">
+      <c r="C91" s="18">
         <f>SPF_growth!K91/100</f>
         <v>8.4682556073343296E-3</v>
       </c>
-      <c r="D91" s="18">
-        <v>2.13</v>
+      <c r="D91" s="20">
+        <v>2.125</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -8625,12 +8626,12 @@
       <c r="B92" s="2">
         <v>37802</v>
       </c>
-      <c r="C92" s="19">
+      <c r="C92" s="18">
         <f>SPF_growth!K92/100</f>
         <v>8.8435084553293297E-3</v>
       </c>
-      <c r="D92" s="18">
-        <v>2.09</v>
+      <c r="D92" s="20">
+        <v>2.0922999999999998</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -8640,12 +8641,12 @@
       <c r="B93" s="2">
         <v>37894</v>
       </c>
-      <c r="C93" s="19">
+      <c r="C93" s="18">
         <f>SPF_growth!K93/100</f>
         <v>9.4749626894177208E-3</v>
       </c>
-      <c r="D93" s="18">
-        <v>1.82</v>
+      <c r="D93" s="20">
+        <v>1.8247</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -8655,12 +8656,12 @@
       <c r="B94" s="2">
         <v>37986</v>
       </c>
-      <c r="C94" s="19">
+      <c r="C94" s="18">
         <f>SPF_growth!K94/100</f>
         <v>9.5437163552321014E-3</v>
       </c>
-      <c r="D94" s="18">
-        <v>2.13</v>
+      <c r="D94" s="20">
+        <v>2.125</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -8670,12 +8671,12 @@
       <c r="B95" s="2">
         <v>38077</v>
       </c>
-      <c r="C95" s="19">
+      <c r="C95" s="18">
         <f>SPF_growth!K95/100</f>
         <v>9.9685873278418935E-3</v>
       </c>
-      <c r="D95" s="18">
-        <v>1.63</v>
+      <c r="D95" s="20">
+        <v>1.6274</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -8685,12 +8686,12 @@
       <c r="B96" s="2">
         <v>38168</v>
       </c>
-      <c r="C96" s="19">
+      <c r="C96" s="18">
         <f>SPF_growth!K96/100</f>
         <v>9.93120631126021E-3</v>
       </c>
-      <c r="D96" s="18">
-        <v>2.13</v>
+      <c r="D96" s="20">
+        <v>2.1318000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -8700,11 +8701,11 @@
       <c r="B97" s="2">
         <v>38260</v>
       </c>
-      <c r="C97" s="19">
+      <c r="C97" s="18">
         <f>SPF_growth!K97/100</f>
         <v>9.256067547759983E-3</v>
       </c>
-      <c r="D97" s="18">
+      <c r="D97" s="20">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -8715,12 +8716,12 @@
       <c r="B98" s="2">
         <v>38352</v>
       </c>
-      <c r="C98" s="19">
+      <c r="C98" s="18">
         <f>SPF_growth!K98/100</f>
         <v>8.4999972112047573E-3</v>
       </c>
-      <c r="D98" s="18">
-        <v>2.2599999999999998</v>
+      <c r="D98" s="20">
+        <v>2.2629999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -8730,11 +8731,11 @@
       <c r="B99" s="2">
         <v>38442</v>
       </c>
-      <c r="C99" s="19">
+      <c r="C99" s="18">
         <f>SPF_growth!K99/100</f>
         <v>8.7124426101865549E-3</v>
       </c>
-      <c r="D99" s="18">
+      <c r="D99" s="20">
         <v>2.25</v>
       </c>
     </row>
@@ -8745,12 +8746,12 @@
       <c r="B100" s="2">
         <v>38533</v>
       </c>
-      <c r="C100" s="19">
+      <c r="C100" s="18">
         <f>SPF_growth!K100/100</f>
         <v>8.462469551814511E-3</v>
       </c>
-      <c r="D100" s="18">
-        <v>2.38</v>
+      <c r="D100" s="20">
+        <v>2.375</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -8760,12 +8761,12 @@
       <c r="B101" s="2">
         <v>38625</v>
       </c>
-      <c r="C101" s="19">
+      <c r="C101" s="18">
         <f>SPF_growth!K101/100</f>
         <v>8.4186884409296336E-3</v>
       </c>
-      <c r="D101" s="18">
-        <v>2.44</v>
+      <c r="D101" s="20">
+        <v>2.4371999999999998</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -8775,12 +8776,12 @@
       <c r="B102" s="2">
         <v>38717</v>
       </c>
-      <c r="C102" s="19">
+      <c r="C102" s="18">
         <f>SPF_growth!K102/100</f>
         <v>8.3686041882338191E-3</v>
       </c>
-      <c r="D102" s="18">
-        <v>2.39</v>
+      <c r="D102" s="20">
+        <v>2.3929999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -8790,12 +8791,12 @@
       <c r="B103" s="2">
         <v>38807</v>
       </c>
-      <c r="C103" s="19">
+      <c r="C103" s="18">
         <f>SPF_growth!K103/100</f>
         <v>8.0436963008880813E-3</v>
       </c>
-      <c r="D103" s="18">
-        <v>2.4300000000000002</v>
+      <c r="D103" s="20">
+        <v>2.4295</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -8805,12 +8806,12 @@
       <c r="B104" s="2">
         <v>38898</v>
       </c>
-      <c r="C104" s="19">
+      <c r="C104" s="18">
         <f>SPF_growth!K104/100</f>
         <v>7.5062325715924416E-3</v>
       </c>
-      <c r="D104" s="18">
-        <v>2.39</v>
+      <c r="D104" s="20">
+        <v>2.3864999999999998</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -8820,12 +8821,12 @@
       <c r="B105" s="2">
         <v>38990</v>
       </c>
-      <c r="C105" s="19">
+      <c r="C105" s="18">
         <f>SPF_growth!K105/100</f>
         <v>7.1499773483414408E-3</v>
       </c>
-      <c r="D105" s="18">
-        <v>2.63</v>
+      <c r="D105" s="20">
+        <v>2.6282999999999999</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -8835,12 +8836,12 @@
       <c r="B106" s="2">
         <v>39082</v>
       </c>
-      <c r="C106" s="19">
+      <c r="C106" s="18">
         <f>SPF_growth!K106/100</f>
         <v>7.1374786656293043E-3</v>
       </c>
-      <c r="D106" s="18">
-        <v>2.62</v>
+      <c r="D106" s="20">
+        <v>2.6179999999999999</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -8850,12 +8851,12 @@
       <c r="B107" s="2">
         <v>39172</v>
       </c>
-      <c r="C107" s="19">
+      <c r="C107" s="18">
         <f>SPF_growth!K107/100</f>
         <v>7.4811657137521248E-3</v>
       </c>
-      <c r="D107" s="18">
-        <v>2.46</v>
+      <c r="D107" s="20">
+        <v>2.4563000000000001</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -8865,12 +8866,12 @@
       <c r="B108" s="2">
         <v>39263</v>
       </c>
-      <c r="C108" s="19">
+      <c r="C108" s="18">
         <f>SPF_growth!K108/100</f>
         <v>7.1061813537347529E-3</v>
       </c>
-      <c r="D108" s="18">
-        <v>2.4300000000000002</v>
+      <c r="D108" s="20">
+        <v>2.4340999999999999</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -8880,12 +8881,12 @@
       <c r="B109" s="2">
         <v>39355</v>
       </c>
-      <c r="C109" s="19">
+      <c r="C109" s="18">
         <f>SPF_growth!K109/100</f>
         <v>6.8312134796624235E-3</v>
       </c>
-      <c r="D109" s="18">
-        <v>2.23</v>
+      <c r="D109" s="20">
+        <v>2.2284999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -8895,12 +8896,12 @@
       <c r="B110" s="2">
         <v>39447</v>
       </c>
-      <c r="C110" s="19">
+      <c r="C110" s="18">
         <f>SPF_growth!K110/100</f>
         <v>6.2310511792726953E-3</v>
       </c>
-      <c r="D110" s="18">
-        <v>2.44</v>
+      <c r="D110" s="20">
+        <v>2.4424000000000001</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -8910,12 +8911,12 @@
       <c r="B111" s="2">
         <v>39538</v>
       </c>
-      <c r="C111" s="19">
+      <c r="C111" s="18">
         <f>SPF_growth!K111/100</f>
         <v>6.2672552093250289E-3</v>
       </c>
-      <c r="D111" s="18">
-        <v>2.38</v>
+      <c r="D111" s="20">
+        <v>2.3818999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -8925,12 +8926,12 @@
       <c r="B112" s="2">
         <v>39629</v>
       </c>
-      <c r="C112" s="19">
+      <c r="C112" s="18">
         <f>SPF_growth!K112/100</f>
         <v>5.2059145264187201E-3</v>
       </c>
-      <c r="D112" s="18">
-        <v>2.67</v>
+      <c r="D112" s="20">
+        <v>2.6650999999999998</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -8940,12 +8941,12 @@
       <c r="B113" s="2">
         <v>39721</v>
       </c>
-      <c r="C113" s="19">
+      <c r="C113" s="18">
         <f>SPF_growth!K113/100</f>
         <v>4.3297974658751404E-3</v>
       </c>
-      <c r="D113" s="18">
-        <v>2.52</v>
+      <c r="D113" s="20">
+        <v>2.5230000000000001</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -8955,12 +8956,12 @@
       <c r="B114" s="2">
         <v>39813</v>
       </c>
-      <c r="C114" s="19">
+      <c r="C114" s="18">
         <f>SPF_growth!K114/100</f>
         <v>1.7892637742296102E-3</v>
       </c>
-      <c r="D114" s="18">
-        <v>1.76</v>
+      <c r="D114" s="20">
+        <v>1.756</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -8970,12 +8971,12 @@
       <c r="B115" s="2">
         <v>39903</v>
       </c>
-      <c r="C115" s="19">
+      <c r="C115" s="18">
         <f>SPF_growth!K115/100</f>
         <v>2.1358213498881007E-3</v>
       </c>
-      <c r="D115" s="18">
-        <v>1.56</v>
+      <c r="D115" s="20">
+        <v>1.5550999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -8985,12 +8986,12 @@
       <c r="B116" s="2">
         <v>39994</v>
       </c>
-      <c r="C116" s="19">
+      <c r="C116" s="18">
         <f>SPF_growth!K116/100</f>
         <v>4.5724672696989543E-3</v>
       </c>
-      <c r="D116" s="18">
-        <v>1.71</v>
+      <c r="D116" s="20">
+        <v>1.7069000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -9000,12 +9001,12 @@
       <c r="B117" s="2">
         <v>40086</v>
       </c>
-      <c r="C117" s="19">
+      <c r="C117" s="18">
         <f>SPF_growth!K117/100</f>
         <v>6.2998367858191351E-3</v>
       </c>
-      <c r="D117" s="18">
-        <v>1.8</v>
+      <c r="D117" s="20">
+        <v>1.8022</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -9015,12 +9016,12 @@
       <c r="B118" s="2">
         <v>40178</v>
       </c>
-      <c r="C118" s="19">
+      <c r="C118" s="18">
         <f>SPF_growth!K118/100</f>
         <v>6.3935801326362451E-3</v>
       </c>
-      <c r="D118" s="18">
-        <v>1.63</v>
+      <c r="D118" s="20">
+        <v>1.6329</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -9030,12 +9031,12 @@
       <c r="B119" s="2">
         <v>40268</v>
       </c>
-      <c r="C119" s="19">
+      <c r="C119" s="18">
         <f>SPF_growth!K119/100</f>
         <v>6.7812494761951836E-3</v>
       </c>
-      <c r="D119" s="18">
-        <v>1.79</v>
+      <c r="D119" s="20">
+        <v>1.7883</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -9045,12 +9046,12 @@
       <c r="B120" s="2">
         <v>40359</v>
       </c>
-      <c r="C120" s="19">
+      <c r="C120" s="18">
         <f>SPF_growth!K120/100</f>
         <v>7.5497999417120099E-3</v>
       </c>
-      <c r="D120" s="18">
-        <v>1.88</v>
+      <c r="D120" s="20">
+        <v>1.8774999999999999</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -9060,12 +9061,12 @@
       <c r="B121" s="2">
         <v>40451</v>
       </c>
-      <c r="C121" s="19">
+      <c r="C121" s="18">
         <f>SPF_growth!K121/100</f>
         <v>6.9809261182789406E-3</v>
       </c>
-      <c r="D121" s="18">
-        <v>1.72</v>
+      <c r="D121" s="20">
+        <v>1.7209000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -9075,12 +9076,12 @@
       <c r="B122" s="2">
         <v>40543</v>
       </c>
-      <c r="C122" s="19">
+      <c r="C122" s="18">
         <f>SPF_growth!K122/100</f>
         <v>7.037163570069227E-3</v>
       </c>
-      <c r="D122" s="18">
-        <v>1.61</v>
+      <c r="D122" s="20">
+        <v>1.609</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -9090,12 +9091,12 @@
       <c r="B123" s="2">
         <v>40633</v>
       </c>
-      <c r="C123" s="19">
+      <c r="C123" s="18">
         <f>SPF_growth!K123/100</f>
         <v>8.1373908181443522E-3</v>
       </c>
-      <c r="D123" s="18">
-        <v>1.72</v>
+      <c r="D123" s="20">
+        <v>1.7246999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -9105,12 +9106,12 @@
       <c r="B124" s="2">
         <v>40724</v>
       </c>
-      <c r="C124" s="19">
+      <c r="C124" s="18">
         <f>SPF_growth!K124/100</f>
         <v>7.6682308294573343E-3</v>
       </c>
-      <c r="D124" s="18">
-        <v>2.13</v>
+      <c r="D124" s="20">
+        <v>2.1303999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -9120,12 +9121,12 @@
       <c r="B125" s="2">
         <v>40816</v>
       </c>
-      <c r="C125" s="19">
+      <c r="C125" s="18">
         <f>SPF_growth!K125/100</f>
         <v>6.7621047359829323E-3</v>
       </c>
-      <c r="D125" s="18">
-        <v>2.0099999999999998</v>
+      <c r="D125" s="20">
+        <v>2.0125000000000002</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -9135,12 +9136,12 @@
       <c r="B126" s="2">
         <v>40908</v>
       </c>
-      <c r="C126" s="19">
+      <c r="C126" s="18">
         <f>SPF_growth!K126/100</f>
         <v>6.4498981568823499E-3</v>
       </c>
-      <c r="D126" s="18">
-        <v>1.97</v>
+      <c r="D126" s="20">
+        <v>1.9692000000000001</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -9150,12 +9151,12 @@
       <c r="B127" s="2">
         <v>40999</v>
       </c>
-      <c r="C127" s="19">
+      <c r="C127" s="18">
         <f>SPF_growth!K127/100</f>
         <v>6.6747721160693718E-3</v>
       </c>
-      <c r="D127" s="18">
-        <v>2.08</v>
+      <c r="D127" s="20">
+        <v>2.0750000000000002</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -9165,12 +9166,12 @@
       <c r="B128" s="2">
         <v>41090</v>
       </c>
-      <c r="C128" s="19">
+      <c r="C128" s="18">
         <f>SPF_growth!K128/100</f>
         <v>6.537478811403874E-3</v>
       </c>
-      <c r="D128" s="18">
-        <v>2.1800000000000002</v>
+      <c r="D128" s="20">
+        <v>2.1831</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -9180,12 +9181,12 @@
       <c r="B129" s="2">
         <v>41182</v>
       </c>
-      <c r="C129" s="19">
+      <c r="C129" s="18">
         <f>SPF_growth!K129/100</f>
         <v>5.5623034792899873E-3</v>
       </c>
-      <c r="D129" s="18">
-        <v>2.11</v>
+      <c r="D129" s="20">
+        <v>2.1097999999999999</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -9195,12 +9196,12 @@
       <c r="B130" s="2">
         <v>41274</v>
       </c>
-      <c r="C130" s="19">
+      <c r="C130" s="18">
         <f>SPF_growth!K130/100</f>
         <v>5.7743478978349305E-3</v>
       </c>
-      <c r="D130" s="18">
-        <v>2.19</v>
+      <c r="D130" s="20">
+        <v>2.1930999999999998</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -9210,11 +9211,11 @@
       <c r="B131" s="2">
         <v>41364</v>
       </c>
-      <c r="C131" s="19">
+      <c r="C131" s="18">
         <f>SPF_growth!K131/100</f>
         <v>6.3249343229643262E-3</v>
       </c>
-      <c r="D131" s="18">
+      <c r="D131" s="20">
         <v>2.1</v>
       </c>
     </row>
@@ -9225,12 +9226,12 @@
       <c r="B132" s="2">
         <v>41455</v>
       </c>
-      <c r="C132" s="19">
+      <c r="C132" s="18">
         <f>SPF_growth!K132/100</f>
         <v>6.6621833905278205E-3</v>
       </c>
-      <c r="D132" s="18">
-        <v>2.04</v>
+      <c r="D132" s="20">
+        <v>2.0413999999999999</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -9240,12 +9241,12 @@
       <c r="B133" s="2">
         <v>41547</v>
       </c>
-      <c r="C133" s="19">
+      <c r="C133" s="18">
         <f>SPF_growth!K133/100</f>
         <v>6.7248360627107928E-3</v>
       </c>
-      <c r="D133" s="18">
-        <v>1.86</v>
+      <c r="D133" s="20">
+        <v>1.8626</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -9255,12 +9256,12 @@
       <c r="B134" s="2">
         <v>41639</v>
       </c>
-      <c r="C134" s="19">
+      <c r="C134" s="18">
         <f>SPF_growth!K134/100</f>
         <v>6.9936364774929594E-3</v>
       </c>
-      <c r="D134" s="18">
-        <v>1.98</v>
+      <c r="D134" s="20">
+        <v>1.984</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -9270,12 +9271,12 @@
       <c r="B135" s="2">
         <v>41729</v>
       </c>
-      <c r="C135" s="19">
+      <c r="C135" s="18">
         <f>SPF_growth!K135/100</f>
         <v>7.343627884191184E-3</v>
       </c>
-      <c r="D135" s="18">
-        <v>1.89</v>
+      <c r="D135" s="20">
+        <v>1.8880999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -9285,12 +9286,12 @@
       <c r="B136" s="2">
         <v>41820</v>
       </c>
-      <c r="C136" s="19">
+      <c r="C136" s="18">
         <f>SPF_growth!K136/100</f>
         <v>7.7436990780379578E-3</v>
       </c>
-      <c r="D136" s="18">
-        <v>1.96</v>
+      <c r="D136" s="20">
+        <v>1.9582999999999999</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -9300,12 +9301,12 @@
       <c r="B137" s="2">
         <v>41912</v>
       </c>
-      <c r="C137" s="19">
+      <c r="C137" s="18">
         <f>SPF_growth!K137/100</f>
         <v>7.6687366054348782E-3</v>
       </c>
-      <c r="D137" s="18">
-        <v>2.1</v>
+      <c r="D137" s="20">
+        <v>2.0990000000000002</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -9315,12 +9316,12 @@
       <c r="B138" s="2">
         <v>42004</v>
       </c>
-      <c r="C138" s="19">
+      <c r="C138" s="18">
         <f>SPF_growth!K138/100</f>
         <v>7.268691307859898E-3</v>
       </c>
-      <c r="D138" s="18">
-        <v>1.92</v>
+      <c r="D138" s="20">
+        <v>1.9161999999999999</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -9330,12 +9331,12 @@
       <c r="B139" s="2">
         <v>42094</v>
       </c>
-      <c r="C139" s="19">
+      <c r="C139" s="18">
         <f>SPF_growth!K139/100</f>
         <v>7.2187159691659009E-3</v>
       </c>
-      <c r="D139" s="18">
-        <v>1.89</v>
+      <c r="D139" s="20">
+        <v>1.8937999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -9345,12 +9346,12 @@
       <c r="B140" s="2">
         <v>42185</v>
       </c>
-      <c r="C140" s="19">
+      <c r="C140" s="18">
         <f>SPF_growth!K140/100</f>
         <v>7.1747712375660466E-3</v>
       </c>
-      <c r="D140" s="18">
-        <v>1.97</v>
+      <c r="D140" s="20">
+        <v>1.9731000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -9360,12 +9361,12 @@
       <c r="B141" s="2">
         <v>42277</v>
       </c>
-      <c r="C141" s="19">
+      <c r="C141" s="18">
         <f>SPF_growth!K141/100</f>
         <v>6.9499970517634679E-3</v>
       </c>
-      <c r="D141" s="18">
-        <v>2.04</v>
+      <c r="D141" s="20">
+        <v>2.0421999999999998</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -9375,12 +9376,12 @@
       <c r="B142" s="2">
         <v>42369</v>
       </c>
-      <c r="C142" s="19">
+      <c r="C142" s="18">
         <f>SPF_growth!K142/100</f>
         <v>6.543647354068538E-3</v>
       </c>
-      <c r="D142" s="18">
-        <v>2.04</v>
+      <c r="D142" s="20">
+        <v>2.0434999999999999</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -9390,12 +9391,12 @@
       <c r="B143" s="2">
         <v>42460</v>
       </c>
-      <c r="C143" s="19">
+      <c r="C143" s="18">
         <f>SPF_growth!K143/100</f>
         <v>6.03122229410058E-3</v>
       </c>
-      <c r="D143" s="18">
-        <v>1.98</v>
+      <c r="D143" s="20">
+        <v>1.9849000000000001</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -9405,12 +9406,12 @@
       <c r="B144" s="2">
         <v>42551</v>
       </c>
-      <c r="C144" s="19">
+      <c r="C144" s="18">
         <f>SPF_growth!K144/100</f>
         <v>5.9687462139725866E-3</v>
       </c>
-      <c r="D144" s="18">
-        <v>2.06</v>
+      <c r="D144" s="20">
+        <v>2.0573999999999999</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -9420,12 +9421,12 @@
       <c r="B145" s="2">
         <v>42643</v>
       </c>
-      <c r="C145" s="19">
+      <c r="C145" s="18">
         <f>SPF_growth!K145/100</f>
         <v>5.6249825964032052E-3</v>
       </c>
-      <c r="D145" s="18">
-        <v>2.23</v>
+      <c r="D145" s="20">
+        <v>2.2275999999999998</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -9435,12 +9436,12 @@
       <c r="B146" s="2">
         <v>42735</v>
       </c>
-      <c r="C146" s="19">
+      <c r="C146" s="18">
         <f>SPF_growth!K146/100</f>
         <v>5.5187463676455994E-3</v>
       </c>
-      <c r="D146" s="18">
-        <v>2.2000000000000002</v>
+      <c r="D146" s="20">
+        <v>2.2029000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -9450,12 +9451,12 @@
       <c r="B147" s="2">
         <v>42825</v>
       </c>
-      <c r="C147" s="19">
+      <c r="C147" s="18">
         <f>SPF_growth!K147/100</f>
         <v>5.8124890472608381E-3</v>
       </c>
-      <c r="D147" s="18">
-        <v>2.36</v>
+      <c r="D147" s="20">
+        <v>2.3595999999999999</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -9465,12 +9466,12 @@
       <c r="B148" s="2">
         <v>42916</v>
       </c>
-      <c r="C148" s="19">
+      <c r="C148" s="18">
         <f>SPF_growth!K148/100</f>
         <v>6.3061991793602612E-3</v>
       </c>
-      <c r="D148" s="18">
-        <v>2.2799999999999998</v>
+      <c r="D148" s="20">
+        <v>2.2749999999999999</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -9480,12 +9481,12 @@
       <c r="B149" s="2">
         <v>43008</v>
       </c>
-      <c r="C149" s="19">
+      <c r="C149" s="18">
         <f>SPF_growth!K149/100</f>
         <v>5.8749818241192742E-3</v>
       </c>
-      <c r="D149" s="18">
-        <v>2.21</v>
+      <c r="D149" s="20">
+        <v>2.2052999999999998</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -9495,12 +9496,12 @@
       <c r="B150" s="2">
         <v>43100</v>
       </c>
-      <c r="C150" s="19">
+      <c r="C150" s="18">
         <f>SPF_growth!K150/100</f>
         <v>5.7937115634378866E-3</v>
       </c>
-      <c r="D150" s="18">
-        <v>2.09</v>
+      <c r="D150" s="20">
+        <v>2.0907</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -9510,12 +9511,12 @@
       <c r="B151" s="2">
         <v>43190</v>
       </c>
-      <c r="C151" s="19">
+      <c r="C151" s="18">
         <f>SPF_growth!K151/100</f>
         <v>6.5998859078126859E-3</v>
       </c>
-      <c r="D151" s="18">
-        <v>2.21</v>
+      <c r="D151" s="20">
+        <v>2.2117</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -9525,12 +9526,12 @@
       <c r="B152" s="2">
         <v>43281</v>
       </c>
-      <c r="C152" s="19">
+      <c r="C152" s="18">
         <f>SPF_growth!K152/100</f>
         <v>6.7373568240012283E-3</v>
       </c>
-      <c r="D152" s="18">
-        <v>2.2599999999999998</v>
+      <c r="D152" s="20">
+        <v>2.2597</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -9540,12 +9541,12 @@
       <c r="B153" s="2">
         <v>43373</v>
       </c>
-      <c r="C153" s="19">
+      <c r="C153" s="18">
         <f>SPF_growth!K153/100</f>
         <v>6.6312159467654119E-3</v>
       </c>
-      <c r="D153" s="18">
-        <v>2.2599999999999998</v>
+      <c r="D153" s="20">
+        <v>2.2589000000000001</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -9555,12 +9556,12 @@
       <c r="B154" s="2">
         <v>43465</v>
       </c>
-      <c r="C154" s="19">
+      <c r="C154" s="18">
         <f>SPF_growth!K154/100</f>
         <v>6.0186597195719393E-3</v>
       </c>
-      <c r="D154" s="18">
-        <v>2.37</v>
+      <c r="D154" s="20">
+        <v>2.3658000000000001</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -9570,12 +9571,12 @@
       <c r="B155" s="2">
         <v>43555</v>
       </c>
-      <c r="C155" s="19">
+      <c r="C155" s="18">
         <f>SPF_growth!K155/100</f>
         <v>5.5562194855705016E-3</v>
       </c>
-      <c r="D155" s="18">
-        <v>2.27</v>
+      <c r="D155" s="20">
+        <v>2.2650999999999999</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -9585,12 +9586,12 @@
       <c r="B156" s="2">
         <v>43646</v>
       </c>
-      <c r="C156" s="19">
+      <c r="C156" s="18">
         <f>SPF_growth!K156/100</f>
         <v>5.0061460695227655E-3</v>
       </c>
-      <c r="D156" s="18">
-        <v>2.09</v>
+      <c r="D156" s="20">
+        <v>2.0855000000000001</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -9600,12 +9601,12 @@
       <c r="B157" s="2">
         <v>43738</v>
       </c>
-      <c r="C157" s="19">
+      <c r="C157" s="18">
         <f>SPF_growth!K157/100</f>
         <v>4.9312488533208576E-3</v>
       </c>
-      <c r="D157" s="18">
-        <v>2.04</v>
+      <c r="D157" s="20">
+        <v>2.0369000000000002</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -9615,12 +9616,12 @@
       <c r="B158" s="2">
         <v>43830</v>
       </c>
-      <c r="C158" s="19">
+      <c r="C158" s="18">
         <f>SPF_growth!K158/100</f>
-        <v>4.4749716883540902E-3</v>
-      </c>
-      <c r="D158" s="18">
-        <v>2.14</v>
+        <v>4.4707222751454445E-3</v>
+      </c>
+      <c r="D158" s="20">
+        <v>2.1383999999999999</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -9630,12 +9631,12 @@
       <c r="B159" s="2">
         <v>43921</v>
       </c>
-      <c r="C159" s="19">
+      <c r="C159" s="18">
         <f>SPF_growth!K159/100</f>
-        <v>5.2749883424711985E-3</v>
-      </c>
-      <c r="D159" s="18">
-        <v>2.16</v>
+        <v>5.2778019665837839E-3</v>
+      </c>
+      <c r="D159" s="20">
+        <v>2.1581999999999999</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -9645,12 +9646,27 @@
       <c r="B160" s="2">
         <v>44012</v>
       </c>
-      <c r="C160" s="19">
+      <c r="C160" s="18">
         <f>SPF_growth!K160/100</f>
-        <v>1.7458158103855315E-2</v>
-      </c>
-      <c r="D160" s="18">
-        <v>1.86</v>
+        <v>1.7457701945593485E-2</v>
+      </c>
+      <c r="D160" s="20">
+        <v>1.859</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="16">
+        <v>20203</v>
+      </c>
+      <c r="B161" s="2">
+        <v>44104</v>
+      </c>
+      <c r="C161" s="18">
+        <f>SPF_growth!K161/100</f>
+        <v>1.1519212755085606E-2</v>
+      </c>
+      <c r="D161" s="20">
+        <v>1.7697000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -9661,7 +9677,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15562,36 +15578,36 @@
         <v>43830</v>
       </c>
       <c r="C158" s="4">
-        <v>1.9</v>
+        <v>1.8978999999999999</v>
       </c>
       <c r="D158" s="4">
-        <v>1.74</v>
+        <v>1.7354000000000001</v>
       </c>
       <c r="E158" s="4">
-        <v>1.66</v>
+        <v>1.6618999999999999</v>
       </c>
       <c r="F158" s="4">
-        <v>1.86</v>
+        <v>1.8580000000000001</v>
       </c>
       <c r="G158" s="15">
         <f t="shared" si="11"/>
-        <v>1.00475</v>
+        <v>1.00474475</v>
       </c>
       <c r="H158" s="15">
         <f t="shared" si="12"/>
-        <v>1.0043500000000001</v>
+        <v>1.0043385</v>
       </c>
       <c r="I158" s="15">
         <f t="shared" si="13"/>
-        <v>1.0041500000000001</v>
+        <v>1.0041547500000001</v>
       </c>
       <c r="J158" s="15">
         <f t="shared" si="14"/>
-        <v>1.00465</v>
+        <v>1.004645</v>
       </c>
       <c r="K158" s="15">
         <f t="shared" si="15"/>
-        <v>0.44749716883540902</v>
+        <v>0.44707222751454445</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -15602,36 +15618,36 @@
         <v>43921</v>
       </c>
       <c r="C159" s="4">
-        <v>2.1</v>
+        <v>2.1049000000000002</v>
       </c>
       <c r="D159" s="4">
-        <v>2.02</v>
+        <v>2.0238999999999998</v>
       </c>
       <c r="E159" s="4">
-        <v>2.13</v>
+        <v>2.1301000000000001</v>
       </c>
       <c r="F159" s="4">
-        <v>2.19</v>
+        <v>2.1856</v>
       </c>
       <c r="G159" s="15">
         <f t="shared" si="11"/>
-        <v>1.00525</v>
+        <v>1.0052622499999999</v>
       </c>
       <c r="H159" s="15">
         <f t="shared" si="12"/>
-        <v>1.00505</v>
+        <v>1.00505975</v>
       </c>
       <c r="I159" s="15">
         <f t="shared" si="13"/>
-        <v>1.005325</v>
+        <v>1.0053252500000001</v>
       </c>
       <c r="J159" s="15">
         <f t="shared" si="14"/>
-        <v>1.0054749999999999</v>
+        <v>1.0054639999999999</v>
       </c>
       <c r="K159" s="15">
         <f t="shared" si="15"/>
-        <v>0.52749883424711985</v>
+        <v>0.52778019665837839</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -15642,36 +15658,76 @@
         <v>44012</v>
       </c>
       <c r="C160" s="4">
-        <v>10.63</v>
+        <v>10.6335</v>
       </c>
       <c r="D160" s="4">
-        <v>6.48</v>
+        <v>6.4775</v>
       </c>
       <c r="E160" s="4">
-        <v>6.76</v>
+        <v>6.7575000000000003</v>
       </c>
       <c r="F160" s="4">
-        <v>4.09</v>
+        <v>4.0907999999999998</v>
       </c>
       <c r="G160" s="15">
         <f t="shared" ref="G160" si="16">1+C160/400</f>
-        <v>1.026575</v>
+        <v>1.0265837499999999</v>
       </c>
       <c r="H160" s="15">
         <f t="shared" ref="H160" si="17">1+D160/400</f>
-        <v>1.0162</v>
+        <v>1.01619375</v>
       </c>
       <c r="I160" s="15">
         <f t="shared" ref="I160" si="18">1+E160/400</f>
-        <v>1.0168999999999999</v>
+        <v>1.0168937499999999</v>
       </c>
       <c r="J160" s="15">
         <f t="shared" ref="J160" si="19">1+F160/400</f>
-        <v>1.0102249999999999</v>
+        <v>1.010227</v>
       </c>
       <c r="K160" s="15">
         <f t="shared" ref="K160" si="20">100*(PRODUCT(G160:J160)^(1/4)-1)</f>
-        <v>1.7458158103855315</v>
+        <v>1.7457701945593485</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="16">
+        <v>20203</v>
+      </c>
+      <c r="B161" s="2">
+        <v>44104</v>
+      </c>
+      <c r="C161" s="4">
+        <v>5.8066000000000004</v>
+      </c>
+      <c r="D161" s="4">
+        <v>5.2343999999999999</v>
+      </c>
+      <c r="E161" s="4">
+        <v>3.8380000000000001</v>
+      </c>
+      <c r="F161" s="4">
+        <v>3.5560999999999998</v>
+      </c>
+      <c r="G161" s="15">
+        <f t="shared" ref="G161" si="21">1+C161/400</f>
+        <v>1.0145165</v>
+      </c>
+      <c r="H161" s="15">
+        <f t="shared" ref="H161" si="22">1+D161/400</f>
+        <v>1.0130859999999999</v>
+      </c>
+      <c r="I161" s="15">
+        <f t="shared" ref="I161" si="23">1+E161/400</f>
+        <v>1.009595</v>
+      </c>
+      <c r="J161" s="15">
+        <f t="shared" ref="J161" si="24">1+F161/400</f>
+        <v>1.0088902500000001</v>
+      </c>
+      <c r="K161" s="15">
+        <f t="shared" ref="K161" si="25">100*(PRODUCT(G161:J161)^(1/4)-1)</f>
+        <v>1.1519212755085606</v>
       </c>
     </row>
   </sheetData>
@@ -15740,7 +15796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="FT1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="GJ1" sqref="GJ1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -15751,8 +15809,8 @@
     <col min="992" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:951" s="20" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:951" s="19" customFormat="1" ht="16" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>647</v>
       </c>
       <c r="B1" s="12">
@@ -16324,6 +16382,12 @@
       </c>
       <c r="GI1" s="13">
         <v>44012</v>
+      </c>
+      <c r="GJ1" s="13">
+        <v>44043</v>
+      </c>
+      <c r="GK1" s="13">
+        <v>44074</v>
       </c>
     </row>
     <row r="2" spans="1:951">
@@ -16899,6 +16963,12 @@
       </c>
       <c r="GI2" s="11">
         <v>44012</v>
+      </c>
+      <c r="GJ2" s="9">
+        <v>44043</v>
+      </c>
+      <c r="GK2" s="9">
+        <v>44074</v>
       </c>
       <c r="ACF2" s="7"/>
       <c r="ACG2" s="7"/>
@@ -17667,6 +17737,9 @@
       <c r="GI3" s="9">
         <v>43966</v>
       </c>
+      <c r="GK3" s="9">
+        <v>44057</v>
+      </c>
       <c r="ACF3" s="7"/>
       <c r="ACG3" s="7"/>
       <c r="ACH3" s="7"/>
@@ -18434,6 +18507,9 @@
       <c r="GI4" s="9">
         <v>43966</v>
       </c>
+      <c r="GK4" s="9">
+        <v>44057</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
New US_local under baseline_iis incl CPI SPF
</commit_message>
<xml_diff>
--- a/models/baseline_iis/data/US_local.xlsx
+++ b/models/baseline_iis/data/US_local.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Documents/Research/Economics/replication-hasenzagl-et-al-2021/models/baseline_iis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95F78E0-7794-8543-93A8-792CA2004AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A2A19-C4E3-5043-A99E-0DE6E1752C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="6" r:id="rId1"/>
@@ -2537,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="G455" sqref="G455"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15"/>
@@ -7685,7 +7685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E169" sqref="E169"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15"/>
   <cols>

</xml_diff>